<commit_message>
Saving multiple worksheet with excel and new study statuses
</commit_message>
<xml_diff>
--- a/IrbAnalyser/study.xlsx
+++ b/IrbAnalyser/study.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>StudyId</t>
   </si>
@@ -127,6 +127,21 @@
   </si>
   <si>
     <t>www.google.com</t>
+  </si>
+  <si>
+    <t>ad</t>
+  </si>
+  <si>
+    <t>McDonald</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>asd@sdf.dd</t>
   </si>
 </sst>
 </file>
@@ -476,15 +491,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA2"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16" customWidth="1"/>
   </cols>
   <sheetData>
@@ -621,10 +637,62 @@
         <v>36</v>
       </c>
     </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4564654</v>
+      </c>
+      <c r="B3">
+        <v>64654</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <v>123465498</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W3">
+        <v>64554</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="V2" r:id="rId1"/>
     <hyperlink ref="X2" r:id="rId2"/>
+    <hyperlink ref="V3" r:id="rId3"/>
+    <hyperlink ref="X3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>